<commit_message>
rectification en-tete output assurance
</commit_message>
<xml_diff>
--- a/donnees/donnees_premierTraitement/assurance/assurances.xlsx
+++ b/donnees/donnees_premierTraitement/assurance/assurances.xlsx
@@ -63,44 +63,74 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="n">
-        <v>510.0</v>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Tarif</t>
+        </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>06</t>
+          <t>Annee</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>2016</t>
-        </is>
-      </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+          <t>Mois</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Jour</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Heure</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Minute</t>
+        </is>
+      </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>Pays</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>BRETAGNE</t>
-        </is>
-      </c>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
+          <t>Region</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Departement</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Commune</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Latitude</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Longitude</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>511.0</v>
+        <v>510.0</v>
       </c>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>07</t>
+          <t>06</t>
         </is>
       </c>
       <c r="C2" s="1" t="inlineStr">
@@ -132,7 +162,7 @@
       </c>
       <c r="B3" s="1" t="inlineStr">
         <is>
-          <t>08</t>
+          <t>07</t>
         </is>
       </c>
       <c r="C3" s="1" t="inlineStr">
@@ -164,7 +194,7 @@
       </c>
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>09</t>
+          <t>08</t>
         </is>
       </c>
       <c r="C4" s="1" t="inlineStr">
@@ -192,11 +222,11 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>508.0</v>
+        <v>511.0</v>
       </c>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>09</t>
         </is>
       </c>
       <c r="C5" s="1" t="inlineStr">
@@ -224,11 +254,11 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>506.0</v>
+        <v>508.0</v>
       </c>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>10</t>
         </is>
       </c>
       <c r="C6" s="1" t="inlineStr">
@@ -256,11 +286,11 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>502.0</v>
+        <v>506.0</v>
       </c>
       <c r="B7" s="1" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="C7" s="1" t="inlineStr">
@@ -288,16 +318,16 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>503.0</v>
+        <v>502.0</v>
       </c>
       <c r="B8" s="1" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>12</t>
         </is>
       </c>
       <c r="C8" s="1" t="inlineStr">
         <is>
-          <t>2017</t>
+          <t>2016</t>
         </is>
       </c>
       <c r="D8" s="1"/>
@@ -320,11 +350,11 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>502.0</v>
+        <v>503.0</v>
       </c>
       <c r="B9" s="1" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>01</t>
         </is>
       </c>
       <c r="C9" s="1" t="inlineStr">
@@ -352,11 +382,11 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>500.0</v>
+        <v>502.0</v>
       </c>
       <c r="B10" s="1" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>02</t>
         </is>
       </c>
       <c r="C10" s="1" t="inlineStr">
@@ -384,11 +414,11 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>498.0</v>
+        <v>500.0</v>
       </c>
       <c r="B11" s="1" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>03</t>
         </is>
       </c>
       <c r="C11" s="1" t="inlineStr">
@@ -416,11 +446,11 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>495.0</v>
+        <v>498.0</v>
       </c>
       <c r="B12" s="1" t="inlineStr">
         <is>
-          <t>05</t>
+          <t>04</t>
         </is>
       </c>
       <c r="C12" s="1" t="inlineStr">
@@ -448,16 +478,16 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>577.0</v>
+        <v>495.0</v>
       </c>
       <c r="B13" s="1" t="inlineStr">
         <is>
-          <t>06</t>
+          <t>05</t>
         </is>
       </c>
       <c r="C13" s="1" t="inlineStr">
         <is>
-          <t>2016</t>
+          <t>2017</t>
         </is>
       </c>
       <c r="D13" s="1"/>
@@ -470,7 +500,7 @@
       </c>
       <c r="H13" s="1" t="inlineStr">
         <is>
-          <t>NORMANDIE</t>
+          <t>BRETAGNE</t>
         </is>
       </c>
       <c r="I13" s="1"/>
@@ -484,7 +514,7 @@
       </c>
       <c r="B14" s="1" t="inlineStr">
         <is>
-          <t>07</t>
+          <t>06</t>
         </is>
       </c>
       <c r="C14" s="1" t="inlineStr">
@@ -512,11 +542,11 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>578.0</v>
+        <v>577.0</v>
       </c>
       <c r="B15" s="1" t="inlineStr">
         <is>
-          <t>08</t>
+          <t>07</t>
         </is>
       </c>
       <c r="C15" s="1" t="inlineStr">
@@ -544,11 +574,11 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>577.0</v>
+        <v>578.0</v>
       </c>
       <c r="B16" s="1" t="inlineStr">
         <is>
-          <t>09</t>
+          <t>08</t>
         </is>
       </c>
       <c r="C16" s="1" t="inlineStr">
@@ -576,11 +606,11 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>576.0</v>
+        <v>577.0</v>
       </c>
       <c r="B17" s="1" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>09</t>
         </is>
       </c>
       <c r="C17" s="1" t="inlineStr">
@@ -612,7 +642,7 @@
       </c>
       <c r="B18" s="1" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>10</t>
         </is>
       </c>
       <c r="C18" s="1" t="inlineStr">
@@ -640,11 +670,11 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>573.0</v>
+        <v>576.0</v>
       </c>
       <c r="B19" s="1" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="C19" s="1" t="inlineStr">
@@ -672,16 +702,16 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>575.0</v>
+        <v>573.0</v>
       </c>
       <c r="B20" s="1" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>12</t>
         </is>
       </c>
       <c r="C20" s="1" t="inlineStr">
         <is>
-          <t>2017</t>
+          <t>2016</t>
         </is>
       </c>
       <c r="D20" s="1"/>
@@ -704,11 +734,11 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>574.0</v>
+        <v>575.0</v>
       </c>
       <c r="B21" s="1" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>01</t>
         </is>
       </c>
       <c r="C21" s="1" t="inlineStr">
@@ -736,11 +766,11 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>570.0</v>
+        <v>574.0</v>
       </c>
       <c r="B22" s="1" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>02</t>
         </is>
       </c>
       <c r="C22" s="1" t="inlineStr">
@@ -768,11 +798,11 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>568.0</v>
+        <v>570.0</v>
       </c>
       <c r="B23" s="1" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>03</t>
         </is>
       </c>
       <c r="C23" s="1" t="inlineStr">
@@ -800,11 +830,11 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>566.0</v>
+        <v>568.0</v>
       </c>
       <c r="B24" s="1" t="inlineStr">
         <is>
-          <t>05</t>
+          <t>04</t>
         </is>
       </c>
       <c r="C24" s="1" t="inlineStr">
@@ -832,16 +862,16 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>606.0</v>
+        <v>566.0</v>
       </c>
       <c r="B25" s="1" t="inlineStr">
         <is>
-          <t>06</t>
+          <t>05</t>
         </is>
       </c>
       <c r="C25" s="1" t="inlineStr">
         <is>
-          <t>2016</t>
+          <t>2017</t>
         </is>
       </c>
       <c r="D25" s="1"/>
@@ -854,7 +884,7 @@
       </c>
       <c r="H25" s="1" t="inlineStr">
         <is>
-          <t>NORD-PAS-DE-CALAIS-PICARDIE</t>
+          <t>NORMANDIE</t>
         </is>
       </c>
       <c r="I25" s="1"/>
@@ -868,7 +898,7 @@
       </c>
       <c r="B26" s="1" t="inlineStr">
         <is>
-          <t>07</t>
+          <t>06</t>
         </is>
       </c>
       <c r="C26" s="1" t="inlineStr">
@@ -896,11 +926,11 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>607.0</v>
+        <v>606.0</v>
       </c>
       <c r="B27" s="1" t="inlineStr">
         <is>
-          <t>08</t>
+          <t>07</t>
         </is>
       </c>
       <c r="C27" s="1" t="inlineStr">
@@ -928,11 +958,11 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>606.0</v>
+        <v>607.0</v>
       </c>
       <c r="B28" s="1" t="inlineStr">
         <is>
-          <t>09</t>
+          <t>08</t>
         </is>
       </c>
       <c r="C28" s="1" t="inlineStr">
@@ -960,11 +990,11 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>605.0</v>
+        <v>606.0</v>
       </c>
       <c r="B29" s="1" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>09</t>
         </is>
       </c>
       <c r="C29" s="1" t="inlineStr">
@@ -992,11 +1022,11 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>603.0</v>
+        <v>605.0</v>
       </c>
       <c r="B30" s="1" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>10</t>
         </is>
       </c>
       <c r="C30" s="1" t="inlineStr">
@@ -1024,11 +1054,11 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>599.0</v>
+        <v>603.0</v>
       </c>
       <c r="B31" s="1" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="C31" s="1" t="inlineStr">
@@ -1056,16 +1086,16 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>602.0</v>
+        <v>599.0</v>
       </c>
       <c r="B32" s="1" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>12</t>
         </is>
       </c>
       <c r="C32" s="1" t="inlineStr">
         <is>
-          <t>2017</t>
+          <t>2016</t>
         </is>
       </c>
       <c r="D32" s="1"/>
@@ -1088,11 +1118,11 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>601.0</v>
+        <v>602.0</v>
       </c>
       <c r="B33" s="1" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>01</t>
         </is>
       </c>
       <c r="C33" s="1" t="inlineStr">
@@ -1120,11 +1150,11 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>599.0</v>
+        <v>601.0</v>
       </c>
       <c r="B34" s="1" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>02</t>
         </is>
       </c>
       <c r="C34" s="1" t="inlineStr">
@@ -1152,11 +1182,11 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>598.0</v>
+        <v>599.0</v>
       </c>
       <c r="B35" s="1" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>03</t>
         </is>
       </c>
       <c r="C35" s="1" t="inlineStr">
@@ -1184,11 +1214,11 @@
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>596.0</v>
+        <v>598.0</v>
       </c>
       <c r="B36" s="1" t="inlineStr">
         <is>
-          <t>05</t>
+          <t>04</t>
         </is>
       </c>
       <c r="C36" s="1" t="inlineStr">
@@ -1216,16 +1246,16 @@
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>526.0</v>
+        <v>596.0</v>
       </c>
       <c r="B37" s="1" t="inlineStr">
         <is>
-          <t>06</t>
+          <t>05</t>
         </is>
       </c>
       <c r="C37" s="1" t="inlineStr">
         <is>
-          <t>2016</t>
+          <t>2017</t>
         </is>
       </c>
       <c r="D37" s="1"/>
@@ -1238,7 +1268,7 @@
       </c>
       <c r="H37" s="1" t="inlineStr">
         <is>
-          <t>PAYS DE LA LOIRE</t>
+          <t>NORD-PAS-DE-CALAIS-PICARDIE</t>
         </is>
       </c>
       <c r="I37" s="1"/>
@@ -1252,7 +1282,7 @@
       </c>
       <c r="B38" s="1" t="inlineStr">
         <is>
-          <t>07</t>
+          <t>06</t>
         </is>
       </c>
       <c r="C38" s="1" t="inlineStr">
@@ -1280,11 +1310,11 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>527.0</v>
+        <v>526.0</v>
       </c>
       <c r="B39" s="1" t="inlineStr">
         <is>
-          <t>08</t>
+          <t>07</t>
         </is>
       </c>
       <c r="C39" s="1" t="inlineStr">
@@ -1312,11 +1342,11 @@
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>526.0</v>
+        <v>527.0</v>
       </c>
       <c r="B40" s="1" t="inlineStr">
         <is>
-          <t>09</t>
+          <t>08</t>
         </is>
       </c>
       <c r="C40" s="1" t="inlineStr">
@@ -1344,11 +1374,11 @@
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>524.0</v>
+        <v>526.0</v>
       </c>
       <c r="B41" s="1" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>09</t>
         </is>
       </c>
       <c r="C41" s="1" t="inlineStr">
@@ -1376,11 +1406,11 @@
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>523.0</v>
+        <v>524.0</v>
       </c>
       <c r="B42" s="1" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>10</t>
         </is>
       </c>
       <c r="C42" s="1" t="inlineStr">
@@ -1408,11 +1438,11 @@
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>518.0</v>
+        <v>523.0</v>
       </c>
       <c r="B43" s="1" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="C43" s="1" t="inlineStr">
@@ -1440,16 +1470,16 @@
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>519.0</v>
+        <v>518.0</v>
       </c>
       <c r="B44" s="1" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>12</t>
         </is>
       </c>
       <c r="C44" s="1" t="inlineStr">
         <is>
-          <t>2017</t>
+          <t>2016</t>
         </is>
       </c>
       <c r="D44" s="1"/>
@@ -1472,11 +1502,11 @@
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>518.0</v>
+        <v>519.0</v>
       </c>
       <c r="B45" s="1" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>01</t>
         </is>
       </c>
       <c r="C45" s="1" t="inlineStr">
@@ -1504,11 +1534,11 @@
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>516.0</v>
+        <v>518.0</v>
       </c>
       <c r="B46" s="1" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>02</t>
         </is>
       </c>
       <c r="C46" s="1" t="inlineStr">
@@ -1536,11 +1566,11 @@
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>515.0</v>
+        <v>516.0</v>
       </c>
       <c r="B47" s="1" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>03</t>
         </is>
       </c>
       <c r="C47" s="1" t="inlineStr">
@@ -1568,11 +1598,11 @@
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>513.0</v>
+        <v>515.0</v>
       </c>
       <c r="B48" s="1" t="inlineStr">
         <is>
-          <t>05</t>
+          <t>04</t>
         </is>
       </c>
       <c r="C48" s="1" t="inlineStr">
@@ -1600,16 +1630,16 @@
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>695.0</v>
+        <v>513.0</v>
       </c>
       <c r="B49" s="1" t="inlineStr">
         <is>
-          <t>06</t>
+          <t>05</t>
         </is>
       </c>
       <c r="C49" s="1" t="inlineStr">
         <is>
-          <t>2016</t>
+          <t>2017</t>
         </is>
       </c>
       <c r="D49" s="1"/>
@@ -1622,7 +1652,7 @@
       </c>
       <c r="H49" s="1" t="inlineStr">
         <is>
-          <t>ILE-DE-FRANCE</t>
+          <t>PAYS DE LA LOIRE</t>
         </is>
       </c>
       <c r="I49" s="1"/>
@@ -1632,11 +1662,11 @@
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>697.0</v>
+        <v>695.0</v>
       </c>
       <c r="B50" s="1" t="inlineStr">
         <is>
-          <t>07</t>
+          <t>06</t>
         </is>
       </c>
       <c r="C50" s="1" t="inlineStr">
@@ -1664,11 +1694,11 @@
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>698.0</v>
+        <v>697.0</v>
       </c>
       <c r="B51" s="1" t="inlineStr">
         <is>
-          <t>08</t>
+          <t>07</t>
         </is>
       </c>
       <c r="C51" s="1" t="inlineStr">
@@ -1700,7 +1730,7 @@
       </c>
       <c r="B52" s="1" t="inlineStr">
         <is>
-          <t>09</t>
+          <t>08</t>
         </is>
       </c>
       <c r="C52" s="1" t="inlineStr">
@@ -1732,7 +1762,7 @@
       </c>
       <c r="B53" s="1" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>09</t>
         </is>
       </c>
       <c r="C53" s="1" t="inlineStr">
@@ -1760,11 +1790,11 @@
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>697.0</v>
+        <v>698.0</v>
       </c>
       <c r="B54" s="1" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>10</t>
         </is>
       </c>
       <c r="C54" s="1" t="inlineStr">
@@ -1792,11 +1822,11 @@
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>694.0</v>
+        <v>697.0</v>
       </c>
       <c r="B55" s="1" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="C55" s="1" t="inlineStr">
@@ -1824,16 +1854,16 @@
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>695.0</v>
+        <v>694.0</v>
       </c>
       <c r="B56" s="1" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>12</t>
         </is>
       </c>
       <c r="C56" s="1" t="inlineStr">
         <is>
-          <t>2017</t>
+          <t>2016</t>
         </is>
       </c>
       <c r="D56" s="1"/>
@@ -1860,7 +1890,7 @@
       </c>
       <c r="B57" s="1" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>01</t>
         </is>
       </c>
       <c r="C57" s="1" t="inlineStr">
@@ -1888,11 +1918,11 @@
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>693.0</v>
+        <v>695.0</v>
       </c>
       <c r="B58" s="1" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>02</t>
         </is>
       </c>
       <c r="C58" s="1" t="inlineStr">
@@ -1920,11 +1950,11 @@
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>691.0</v>
+        <v>693.0</v>
       </c>
       <c r="B59" s="1" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>03</t>
         </is>
       </c>
       <c r="C59" s="1" t="inlineStr">
@@ -1952,11 +1982,11 @@
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>689.0</v>
+        <v>691.0</v>
       </c>
       <c r="B60" s="1" t="inlineStr">
         <is>
-          <t>05</t>
+          <t>04</t>
         </is>
       </c>
       <c r="C60" s="1" t="inlineStr">
@@ -1984,16 +2014,16 @@
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>553.0</v>
+        <v>689.0</v>
       </c>
       <c r="B61" s="1" t="inlineStr">
         <is>
-          <t>06</t>
+          <t>05</t>
         </is>
       </c>
       <c r="C61" s="1" t="inlineStr">
         <is>
-          <t>2016</t>
+          <t>2017</t>
         </is>
       </c>
       <c r="D61" s="1"/>
@@ -2006,7 +2036,7 @@
       </c>
       <c r="H61" s="1" t="inlineStr">
         <is>
-          <t>CENTRE-VAL DE LOIRE</t>
+          <t>ILE-DE-FRANCE</t>
         </is>
       </c>
       <c r="I61" s="1"/>
@@ -2020,7 +2050,7 @@
       </c>
       <c r="B62" s="1" t="inlineStr">
         <is>
-          <t>07</t>
+          <t>06</t>
         </is>
       </c>
       <c r="C62" s="1" t="inlineStr">
@@ -2048,11 +2078,11 @@
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>554.0</v>
+        <v>553.0</v>
       </c>
       <c r="B63" s="1" t="inlineStr">
         <is>
-          <t>08</t>
+          <t>07</t>
         </is>
       </c>
       <c r="C63" s="1" t="inlineStr">
@@ -2084,7 +2114,7 @@
       </c>
       <c r="B64" s="1" t="inlineStr">
         <is>
-          <t>09</t>
+          <t>08</t>
         </is>
       </c>
       <c r="C64" s="1" t="inlineStr">
@@ -2116,7 +2146,7 @@
       </c>
       <c r="B65" s="1" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>09</t>
         </is>
       </c>
       <c r="C65" s="1" t="inlineStr">
@@ -2148,7 +2178,7 @@
       </c>
       <c r="B66" s="1" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>10</t>
         </is>
       </c>
       <c r="C66" s="1" t="inlineStr">
@@ -2176,11 +2206,11 @@
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>550.0</v>
+        <v>554.0</v>
       </c>
       <c r="B67" s="1" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="C67" s="1" t="inlineStr">
@@ -2208,16 +2238,16 @@
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>553.0</v>
+        <v>550.0</v>
       </c>
       <c r="B68" s="1" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>12</t>
         </is>
       </c>
       <c r="C68" s="1" t="inlineStr">
         <is>
-          <t>2017</t>
+          <t>2016</t>
         </is>
       </c>
       <c r="D68" s="1"/>
@@ -2240,11 +2270,11 @@
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>552.0</v>
+        <v>553.0</v>
       </c>
       <c r="B69" s="1" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>01</t>
         </is>
       </c>
       <c r="C69" s="1" t="inlineStr">
@@ -2272,11 +2302,11 @@
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>549.0</v>
+        <v>552.0</v>
       </c>
       <c r="B70" s="1" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>02</t>
         </is>
       </c>
       <c r="C70" s="1" t="inlineStr">
@@ -2304,11 +2334,11 @@
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
-        <v>548.0</v>
+        <v>549.0</v>
       </c>
       <c r="B71" s="1" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>03</t>
         </is>
       </c>
       <c r="C71" s="1" t="inlineStr">
@@ -2336,11 +2366,11 @@
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
-        <v>546.0</v>
+        <v>548.0</v>
       </c>
       <c r="B72" s="1" t="inlineStr">
         <is>
-          <t>05</t>
+          <t>04</t>
         </is>
       </c>
       <c r="C72" s="1" t="inlineStr">
@@ -2368,16 +2398,16 @@
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
-        <v>558.0</v>
+        <v>546.0</v>
       </c>
       <c r="B73" s="1" t="inlineStr">
         <is>
-          <t>06</t>
+          <t>05</t>
         </is>
       </c>
       <c r="C73" s="1" t="inlineStr">
         <is>
-          <t>2016</t>
+          <t>2017</t>
         </is>
       </c>
       <c r="D73" s="1"/>
@@ -2390,7 +2420,7 @@
       </c>
       <c r="H73" s="1" t="inlineStr">
         <is>
-          <t>BOURGOGNE-FRANCHE-COMTÉ</t>
+          <t>CENTRE-VAL DE LOIRE</t>
         </is>
       </c>
       <c r="I73" s="1"/>
@@ -2404,7 +2434,7 @@
       </c>
       <c r="B74" s="1" t="inlineStr">
         <is>
-          <t>07</t>
+          <t>06</t>
         </is>
       </c>
       <c r="C74" s="1" t="inlineStr">
@@ -2432,11 +2462,11 @@
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
-        <v>557.0</v>
+        <v>558.0</v>
       </c>
       <c r="B75" s="1" t="inlineStr">
         <is>
-          <t>08</t>
+          <t>07</t>
         </is>
       </c>
       <c r="C75" s="1" t="inlineStr">
@@ -2464,11 +2494,11 @@
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
-        <v>556.0</v>
+        <v>557.0</v>
       </c>
       <c r="B76" s="1" t="inlineStr">
         <is>
-          <t>09</t>
+          <t>08</t>
         </is>
       </c>
       <c r="C76" s="1" t="inlineStr">
@@ -2496,11 +2526,11 @@
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
-        <v>555.0</v>
+        <v>556.0</v>
       </c>
       <c r="B77" s="1" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>09</t>
         </is>
       </c>
       <c r="C77" s="1" t="inlineStr">
@@ -2528,11 +2558,11 @@
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
-        <v>554.0</v>
+        <v>555.0</v>
       </c>
       <c r="B78" s="1" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>10</t>
         </is>
       </c>
       <c r="C78" s="1" t="inlineStr">
@@ -2560,11 +2590,11 @@
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
-        <v>550.0</v>
+        <v>554.0</v>
       </c>
       <c r="B79" s="1" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="C79" s="1" t="inlineStr">
@@ -2592,16 +2622,16 @@
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
-        <v>551.0</v>
+        <v>550.0</v>
       </c>
       <c r="B80" s="1" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>12</t>
         </is>
       </c>
       <c r="C80" s="1" t="inlineStr">
         <is>
-          <t>2017</t>
+          <t>2016</t>
         </is>
       </c>
       <c r="D80" s="1"/>
@@ -2628,7 +2658,7 @@
       </c>
       <c r="B81" s="1" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>01</t>
         </is>
       </c>
       <c r="C81" s="1" t="inlineStr">
@@ -2656,11 +2686,11 @@
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
-        <v>548.0</v>
+        <v>551.0</v>
       </c>
       <c r="B82" s="1" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>02</t>
         </is>
       </c>
       <c r="C82" s="1" t="inlineStr">
@@ -2692,7 +2722,7 @@
       </c>
       <c r="B83" s="1" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>03</t>
         </is>
       </c>
       <c r="C83" s="1" t="inlineStr">
@@ -2720,11 +2750,11 @@
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
-        <v>546.0</v>
+        <v>548.0</v>
       </c>
       <c r="B84" s="1" t="inlineStr">
         <is>
-          <t>05</t>
+          <t>04</t>
         </is>
       </c>
       <c r="C84" s="1" t="inlineStr">
@@ -2752,16 +2782,16 @@
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
-        <v>581.0</v>
+        <v>546.0</v>
       </c>
       <c r="B85" s="1" t="inlineStr">
         <is>
-          <t>06</t>
+          <t>05</t>
         </is>
       </c>
       <c r="C85" s="1" t="inlineStr">
         <is>
-          <t>2016</t>
+          <t>2017</t>
         </is>
       </c>
       <c r="D85" s="1"/>
@@ -2774,7 +2804,7 @@
       </c>
       <c r="H85" s="1" t="inlineStr">
         <is>
-          <t>ALSACE-CHAMPAGNE-ARDENNE-LORRAINE</t>
+          <t>BOURGOGNE-FRANCHE-COMTÉ</t>
         </is>
       </c>
       <c r="I85" s="1"/>
@@ -2788,7 +2818,7 @@
       </c>
       <c r="B86" s="1" t="inlineStr">
         <is>
-          <t>07</t>
+          <t>06</t>
         </is>
       </c>
       <c r="C86" s="1" t="inlineStr">
@@ -2816,11 +2846,11 @@
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
-        <v>582.0</v>
+        <v>581.0</v>
       </c>
       <c r="B87" s="1" t="inlineStr">
         <is>
-          <t>08</t>
+          <t>07</t>
         </is>
       </c>
       <c r="C87" s="1" t="inlineStr">
@@ -2852,7 +2882,7 @@
       </c>
       <c r="B88" s="1" t="inlineStr">
         <is>
-          <t>09</t>
+          <t>08</t>
         </is>
       </c>
       <c r="C88" s="1" t="inlineStr">
@@ -2880,11 +2910,11 @@
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
-        <v>580.0</v>
+        <v>582.0</v>
       </c>
       <c r="B89" s="1" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>09</t>
         </is>
       </c>
       <c r="C89" s="1" t="inlineStr">
@@ -2912,11 +2942,11 @@
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
-        <v>578.0</v>
+        <v>580.0</v>
       </c>
       <c r="B90" s="1" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>10</t>
         </is>
       </c>
       <c r="C90" s="1" t="inlineStr">
@@ -2944,11 +2974,11 @@
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
-        <v>574.0</v>
+        <v>578.0</v>
       </c>
       <c r="B91" s="1" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="C91" s="1" t="inlineStr">
@@ -2976,16 +3006,16 @@
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
-        <v>576.0</v>
+        <v>574.0</v>
       </c>
       <c r="B92" s="1" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>12</t>
         </is>
       </c>
       <c r="C92" s="1" t="inlineStr">
         <is>
-          <t>2017</t>
+          <t>2016</t>
         </is>
       </c>
       <c r="D92" s="1"/>
@@ -3012,7 +3042,7 @@
       </c>
       <c r="B93" s="1" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>01</t>
         </is>
       </c>
       <c r="C93" s="1" t="inlineStr">
@@ -3040,11 +3070,11 @@
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
-        <v>574.0</v>
+        <v>576.0</v>
       </c>
       <c r="B94" s="1" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>02</t>
         </is>
       </c>
       <c r="C94" s="1" t="inlineStr">
@@ -3072,11 +3102,11 @@
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
-        <v>573.0</v>
+        <v>574.0</v>
       </c>
       <c r="B95" s="1" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>03</t>
         </is>
       </c>
       <c r="C95" s="1" t="inlineStr">
@@ -3104,11 +3134,11 @@
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
-        <v>570.0</v>
+        <v>573.0</v>
       </c>
       <c r="B96" s="1" t="inlineStr">
         <is>
-          <t>05</t>
+          <t>04</t>
         </is>
       </c>
       <c r="C96" s="1" t="inlineStr">
@@ -3136,16 +3166,16 @@
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
-        <v>549.0</v>
+        <v>570.0</v>
       </c>
       <c r="B97" s="1" t="inlineStr">
         <is>
-          <t>06</t>
+          <t>05</t>
         </is>
       </c>
       <c r="C97" s="1" t="inlineStr">
         <is>
-          <t>2016</t>
+          <t>2017</t>
         </is>
       </c>
       <c r="D97" s="1"/>
@@ -3158,7 +3188,7 @@
       </c>
       <c r="H97" s="1" t="inlineStr">
         <is>
-          <t>AQUITAINE-LIMOUSIN-POITOU-CHARENTES</t>
+          <t>ALSACE-CHAMPAGNE-ARDENNE-LORRAINE</t>
         </is>
       </c>
       <c r="I97" s="1"/>
@@ -3168,11 +3198,11 @@
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
-        <v>548.0</v>
+        <v>549.0</v>
       </c>
       <c r="B98" s="1" t="inlineStr">
         <is>
-          <t>07</t>
+          <t>06</t>
         </is>
       </c>
       <c r="C98" s="1" t="inlineStr">
@@ -3204,7 +3234,7 @@
       </c>
       <c r="B99" s="1" t="inlineStr">
         <is>
-          <t>08</t>
+          <t>07</t>
         </is>
       </c>
       <c r="C99" s="1" t="inlineStr">
@@ -3236,7 +3266,7 @@
       </c>
       <c r="B100" s="1" t="inlineStr">
         <is>
-          <t>09</t>
+          <t>08</t>
         </is>
       </c>
       <c r="C100" s="1" t="inlineStr">
@@ -3264,11 +3294,11 @@
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
-        <v>547.0</v>
+        <v>548.0</v>
       </c>
       <c r="B101" s="1" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>09</t>
         </is>
       </c>
       <c r="C101" s="1" t="inlineStr">
@@ -3296,11 +3326,11 @@
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
-        <v>546.0</v>
+        <v>547.0</v>
       </c>
       <c r="B102" s="1" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>10</t>
         </is>
       </c>
       <c r="C102" s="1" t="inlineStr">
@@ -3328,11 +3358,11 @@
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
-        <v>542.0</v>
+        <v>546.0</v>
       </c>
       <c r="B103" s="1" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="C103" s="1" t="inlineStr">
@@ -3360,16 +3390,16 @@
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
-        <v>543.0</v>
+        <v>542.0</v>
       </c>
       <c r="B104" s="1" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>12</t>
         </is>
       </c>
       <c r="C104" s="1" t="inlineStr">
         <is>
-          <t>2017</t>
+          <t>2016</t>
         </is>
       </c>
       <c r="D104" s="1"/>
@@ -3396,7 +3426,7 @@
       </c>
       <c r="B105" s="1" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>01</t>
         </is>
       </c>
       <c r="C105" s="1" t="inlineStr">
@@ -3424,11 +3454,11 @@
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
-        <v>541.0</v>
+        <v>543.0</v>
       </c>
       <c r="B106" s="1" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>02</t>
         </is>
       </c>
       <c r="C106" s="1" t="inlineStr">
@@ -3456,11 +3486,11 @@
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
-        <v>540.0</v>
+        <v>541.0</v>
       </c>
       <c r="B107" s="1" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>03</t>
         </is>
       </c>
       <c r="C107" s="1" t="inlineStr">
@@ -3488,11 +3518,11 @@
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
-        <v>539.0</v>
+        <v>540.0</v>
       </c>
       <c r="B108" s="1" t="inlineStr">
         <is>
-          <t>05</t>
+          <t>04</t>
         </is>
       </c>
       <c r="C108" s="1" t="inlineStr">
@@ -3520,16 +3550,16 @@
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
-        <v>588.0</v>
+        <v>539.0</v>
       </c>
       <c r="B109" s="1" t="inlineStr">
         <is>
-          <t>06</t>
+          <t>05</t>
         </is>
       </c>
       <c r="C109" s="1" t="inlineStr">
         <is>
-          <t>2016</t>
+          <t>2017</t>
         </is>
       </c>
       <c r="D109" s="1"/>
@@ -3542,7 +3572,7 @@
       </c>
       <c r="H109" s="1" t="inlineStr">
         <is>
-          <t>LANGUEDOC-ROUSSILLON-MIDI-PYRÉNÉES</t>
+          <t>AQUITAINE-LIMOUSIN-POITOU-CHARENTES</t>
         </is>
       </c>
       <c r="I109" s="1"/>
@@ -3556,7 +3586,7 @@
       </c>
       <c r="B110" s="1" t="inlineStr">
         <is>
-          <t>07</t>
+          <t>06</t>
         </is>
       </c>
       <c r="C110" s="1" t="inlineStr">
@@ -3588,7 +3618,7 @@
       </c>
       <c r="B111" s="1" t="inlineStr">
         <is>
-          <t>08</t>
+          <t>07</t>
         </is>
       </c>
       <c r="C111" s="1" t="inlineStr">
@@ -3616,11 +3646,11 @@
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
-        <v>587.0</v>
+        <v>588.0</v>
       </c>
       <c r="B112" s="1" t="inlineStr">
         <is>
-          <t>09</t>
+          <t>08</t>
         </is>
       </c>
       <c r="C112" s="1" t="inlineStr">
@@ -3648,11 +3678,11 @@
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
-        <v>586.0</v>
+        <v>587.0</v>
       </c>
       <c r="B113" s="1" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>09</t>
         </is>
       </c>
       <c r="C113" s="1" t="inlineStr">
@@ -3680,11 +3710,11 @@
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
-        <v>585.0</v>
+        <v>586.0</v>
       </c>
       <c r="B114" s="1" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>10</t>
         </is>
       </c>
       <c r="C114" s="1" t="inlineStr">
@@ -3712,11 +3742,11 @@
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
-        <v>580.0</v>
+        <v>585.0</v>
       </c>
       <c r="B115" s="1" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="C115" s="1" t="inlineStr">
@@ -3744,16 +3774,16 @@
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
-        <v>581.0</v>
+        <v>580.0</v>
       </c>
       <c r="B116" s="1" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>12</t>
         </is>
       </c>
       <c r="C116" s="1" t="inlineStr">
         <is>
-          <t>2017</t>
+          <t>2016</t>
         </is>
       </c>
       <c r="D116" s="1"/>
@@ -3780,7 +3810,7 @@
       </c>
       <c r="B117" s="1" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>01</t>
         </is>
       </c>
       <c r="C117" s="1" t="inlineStr">
@@ -3808,11 +3838,11 @@
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
-        <v>579.0</v>
+        <v>581.0</v>
       </c>
       <c r="B118" s="1" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>02</t>
         </is>
       </c>
       <c r="C118" s="1" t="inlineStr">
@@ -3840,11 +3870,11 @@
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
-        <v>578.0</v>
+        <v>579.0</v>
       </c>
       <c r="B119" s="1" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>03</t>
         </is>
       </c>
       <c r="C119" s="1" t="inlineStr">
@@ -3872,11 +3902,11 @@
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
-        <v>576.0</v>
+        <v>578.0</v>
       </c>
       <c r="B120" s="1" t="inlineStr">
         <is>
-          <t>05</t>
+          <t>04</t>
         </is>
       </c>
       <c r="C120" s="1" t="inlineStr">
@@ -3904,16 +3934,16 @@
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
-        <v>614.0</v>
+        <v>576.0</v>
       </c>
       <c r="B121" s="1" t="inlineStr">
         <is>
-          <t>06</t>
+          <t>05</t>
         </is>
       </c>
       <c r="C121" s="1" t="inlineStr">
         <is>
-          <t>2016</t>
+          <t>2017</t>
         </is>
       </c>
       <c r="D121" s="1"/>
@@ -3926,7 +3956,7 @@
       </c>
       <c r="H121" s="1" t="inlineStr">
         <is>
-          <t>AUVERGNE-RHONE-ALPES</t>
+          <t>LANGUEDOC-ROUSSILLON-MIDI-PYRÉNÉES</t>
         </is>
       </c>
       <c r="I121" s="1"/>
@@ -3940,7 +3970,7 @@
       </c>
       <c r="B122" s="1" t="inlineStr">
         <is>
-          <t>07</t>
+          <t>06</t>
         </is>
       </c>
       <c r="C122" s="1" t="inlineStr">
@@ -3972,7 +4002,7 @@
       </c>
       <c r="B123" s="1" t="inlineStr">
         <is>
-          <t>08</t>
+          <t>07</t>
         </is>
       </c>
       <c r="C123" s="1" t="inlineStr">
@@ -4000,11 +4030,11 @@
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
-        <v>613.0</v>
+        <v>614.0</v>
       </c>
       <c r="B124" s="1" t="inlineStr">
         <is>
-          <t>09</t>
+          <t>08</t>
         </is>
       </c>
       <c r="C124" s="1" t="inlineStr">
@@ -4032,11 +4062,11 @@
     </row>
     <row r="125">
       <c r="A125" s="1" t="n">
-        <v>611.0</v>
+        <v>613.0</v>
       </c>
       <c r="B125" s="1" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>09</t>
         </is>
       </c>
       <c r="C125" s="1" t="inlineStr">
@@ -4064,11 +4094,11 @@
     </row>
     <row r="126">
       <c r="A126" s="1" t="n">
-        <v>609.0</v>
+        <v>611.0</v>
       </c>
       <c r="B126" s="1" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>10</t>
         </is>
       </c>
       <c r="C126" s="1" t="inlineStr">
@@ -4096,11 +4126,11 @@
     </row>
     <row r="127">
       <c r="A127" s="1" t="n">
-        <v>604.0</v>
+        <v>609.0</v>
       </c>
       <c r="B127" s="1" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="C127" s="1" t="inlineStr">
@@ -4128,16 +4158,16 @@
     </row>
     <row r="128">
       <c r="A128" s="1" t="n">
-        <v>605.0</v>
+        <v>604.0</v>
       </c>
       <c r="B128" s="1" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>12</t>
         </is>
       </c>
       <c r="C128" s="1" t="inlineStr">
         <is>
-          <t>2017</t>
+          <t>2016</t>
         </is>
       </c>
       <c r="D128" s="1"/>
@@ -4164,7 +4194,7 @@
       </c>
       <c r="B129" s="1" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>01</t>
         </is>
       </c>
       <c r="C129" s="1" t="inlineStr">
@@ -4192,11 +4222,11 @@
     </row>
     <row r="130">
       <c r="A130" s="1" t="n">
-        <v>604.0</v>
+        <v>605.0</v>
       </c>
       <c r="B130" s="1" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>02</t>
         </is>
       </c>
       <c r="C130" s="1" t="inlineStr">
@@ -4224,11 +4254,11 @@
     </row>
     <row r="131">
       <c r="A131" s="1" t="n">
-        <v>603.0</v>
+        <v>604.0</v>
       </c>
       <c r="B131" s="1" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>03</t>
         </is>
       </c>
       <c r="C131" s="1" t="inlineStr">
@@ -4256,11 +4286,11 @@
     </row>
     <row r="132">
       <c r="A132" s="1" t="n">
-        <v>602.0</v>
+        <v>603.0</v>
       </c>
       <c r="B132" s="1" t="inlineStr">
         <is>
-          <t>05</t>
+          <t>04</t>
         </is>
       </c>
       <c r="C132" s="1" t="inlineStr">
@@ -4288,16 +4318,16 @@
     </row>
     <row r="133">
       <c r="A133" s="1" t="n">
-        <v>696.0</v>
+        <v>602.0</v>
       </c>
       <c r="B133" s="1" t="inlineStr">
         <is>
-          <t>06</t>
+          <t>05</t>
         </is>
       </c>
       <c r="C133" s="1" t="inlineStr">
         <is>
-          <t>2016</t>
+          <t>2017</t>
         </is>
       </c>
       <c r="D133" s="1"/>
@@ -4310,7 +4340,7 @@
       </c>
       <c r="H133" s="1" t="inlineStr">
         <is>
-          <t>PROVENCE-ALPES-COTE D'AZUR</t>
+          <t>AUVERGNE-RHONE-ALPES</t>
         </is>
       </c>
       <c r="I133" s="1"/>
@@ -4320,11 +4350,11 @@
     </row>
     <row r="134">
       <c r="A134" s="1" t="n">
-        <v>697.0</v>
+        <v>696.0</v>
       </c>
       <c r="B134" s="1" t="inlineStr">
         <is>
-          <t>07</t>
+          <t>06</t>
         </is>
       </c>
       <c r="C134" s="1" t="inlineStr">
@@ -4352,11 +4382,11 @@
     </row>
     <row r="135">
       <c r="A135" s="1" t="n">
-        <v>698.0</v>
+        <v>697.0</v>
       </c>
       <c r="B135" s="1" t="inlineStr">
         <is>
-          <t>08</t>
+          <t>07</t>
         </is>
       </c>
       <c r="C135" s="1" t="inlineStr">
@@ -4384,11 +4414,11 @@
     </row>
     <row r="136">
       <c r="A136" s="1" t="n">
-        <v>697.0</v>
+        <v>698.0</v>
       </c>
       <c r="B136" s="1" t="inlineStr">
         <is>
-          <t>09</t>
+          <t>08</t>
         </is>
       </c>
       <c r="C136" s="1" t="inlineStr">
@@ -4420,7 +4450,7 @@
       </c>
       <c r="B137" s="1" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>09</t>
         </is>
       </c>
       <c r="C137" s="1" t="inlineStr">
@@ -4448,11 +4478,11 @@
     </row>
     <row r="138">
       <c r="A138" s="1" t="n">
-        <v>696.0</v>
+        <v>697.0</v>
       </c>
       <c r="B138" s="1" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>10</t>
         </is>
       </c>
       <c r="C138" s="1" t="inlineStr">
@@ -4480,11 +4510,11 @@
     </row>
     <row r="139">
       <c r="A139" s="1" t="n">
-        <v>691.0</v>
+        <v>696.0</v>
       </c>
       <c r="B139" s="1" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="C139" s="1" t="inlineStr">
@@ -4512,16 +4542,16 @@
     </row>
     <row r="140">
       <c r="A140" s="1" t="n">
-        <v>692.0</v>
+        <v>691.0</v>
       </c>
       <c r="B140" s="1" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>12</t>
         </is>
       </c>
       <c r="C140" s="1" t="inlineStr">
         <is>
-          <t>2017</t>
+          <t>2016</t>
         </is>
       </c>
       <c r="D140" s="1"/>
@@ -4544,11 +4574,11 @@
     </row>
     <row r="141">
       <c r="A141" s="1" t="n">
-        <v>693.0</v>
+        <v>692.0</v>
       </c>
       <c r="B141" s="1" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>01</t>
         </is>
       </c>
       <c r="C141" s="1" t="inlineStr">
@@ -4576,11 +4606,11 @@
     </row>
     <row r="142">
       <c r="A142" s="1" t="n">
-        <v>691.0</v>
+        <v>693.0</v>
       </c>
       <c r="B142" s="1" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>02</t>
         </is>
       </c>
       <c r="C142" s="1" t="inlineStr">
@@ -4608,11 +4638,11 @@
     </row>
     <row r="143">
       <c r="A143" s="1" t="n">
-        <v>690.0</v>
+        <v>691.0</v>
       </c>
       <c r="B143" s="1" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>03</t>
         </is>
       </c>
       <c r="C143" s="1" t="inlineStr">
@@ -4640,11 +4670,11 @@
     </row>
     <row r="144">
       <c r="A144" s="1" t="n">
-        <v>687.0</v>
+        <v>690.0</v>
       </c>
       <c r="B144" s="1" t="inlineStr">
         <is>
-          <t>05</t>
+          <t>04</t>
         </is>
       </c>
       <c r="C144" s="1" t="inlineStr">
@@ -4672,16 +4702,16 @@
     </row>
     <row r="145">
       <c r="A145" s="1" t="n">
-        <v>566.0</v>
+        <v>687.0</v>
       </c>
       <c r="B145" s="1" t="inlineStr">
         <is>
-          <t>06</t>
+          <t>05</t>
         </is>
       </c>
       <c r="C145" s="1" t="inlineStr">
         <is>
-          <t>2016</t>
+          <t>2017</t>
         </is>
       </c>
       <c r="D145" s="1"/>
@@ -4694,7 +4724,7 @@
       </c>
       <c r="H145" s="1" t="inlineStr">
         <is>
-          <t>CORSE</t>
+          <t>PROVENCE-ALPES-COTE D'AZUR</t>
         </is>
       </c>
       <c r="I145" s="1"/>
@@ -4704,11 +4734,11 @@
     </row>
     <row r="146">
       <c r="A146" s="1" t="n">
-        <v>562.0</v>
+        <v>566.0</v>
       </c>
       <c r="B146" s="1" t="inlineStr">
         <is>
-          <t>07</t>
+          <t>06</t>
         </is>
       </c>
       <c r="C146" s="1" t="inlineStr">
@@ -4740,7 +4770,7 @@
       </c>
       <c r="B147" s="1" t="inlineStr">
         <is>
-          <t>08</t>
+          <t>07</t>
         </is>
       </c>
       <c r="C147" s="1" t="inlineStr">
@@ -4768,11 +4798,11 @@
     </row>
     <row r="148">
       <c r="A148" s="1" t="n">
-        <v>558.0</v>
+        <v>562.0</v>
       </c>
       <c r="B148" s="1" t="inlineStr">
         <is>
-          <t>09</t>
+          <t>08</t>
         </is>
       </c>
       <c r="C148" s="1" t="inlineStr">
@@ -4800,11 +4830,11 @@
     </row>
     <row r="149">
       <c r="A149" s="1" t="n">
-        <v>555.0</v>
+        <v>558.0</v>
       </c>
       <c r="B149" s="1" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>09</t>
         </is>
       </c>
       <c r="C149" s="1" t="inlineStr">
@@ -4832,11 +4862,11 @@
     </row>
     <row r="150">
       <c r="A150" s="1" t="n">
-        <v>553.0</v>
+        <v>555.0</v>
       </c>
       <c r="B150" s="1" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>10</t>
         </is>
       </c>
       <c r="C150" s="1" t="inlineStr">
@@ -4864,11 +4894,11 @@
     </row>
     <row r="151">
       <c r="A151" s="1" t="n">
-        <v>547.0</v>
+        <v>553.0</v>
       </c>
       <c r="B151" s="1" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="C151" s="1" t="inlineStr">
@@ -4896,16 +4926,16 @@
     </row>
     <row r="152">
       <c r="A152" s="1" t="n">
-        <v>548.0</v>
+        <v>547.0</v>
       </c>
       <c r="B152" s="1" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>12</t>
         </is>
       </c>
       <c r="C152" s="1" t="inlineStr">
         <is>
-          <t>2017</t>
+          <t>2016</t>
         </is>
       </c>
       <c r="D152" s="1"/>
@@ -4928,11 +4958,11 @@
     </row>
     <row r="153">
       <c r="A153" s="1" t="n">
-        <v>544.0</v>
+        <v>548.0</v>
       </c>
       <c r="B153" s="1" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>01</t>
         </is>
       </c>
       <c r="C153" s="1" t="inlineStr">
@@ -4960,11 +4990,11 @@
     </row>
     <row r="154">
       <c r="A154" s="1" t="n">
-        <v>538.0</v>
+        <v>544.0</v>
       </c>
       <c r="B154" s="1" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>02</t>
         </is>
       </c>
       <c r="C154" s="1" t="inlineStr">
@@ -4992,11 +5022,11 @@
     </row>
     <row r="155">
       <c r="A155" s="1" t="n">
-        <v>534.0</v>
+        <v>538.0</v>
       </c>
       <c r="B155" s="1" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>03</t>
         </is>
       </c>
       <c r="C155" s="1" t="inlineStr">
@@ -5024,11 +5054,11 @@
     </row>
     <row r="156">
       <c r="A156" s="1" t="n">
-        <v>531.0</v>
+        <v>534.0</v>
       </c>
       <c r="B156" s="1" t="inlineStr">
         <is>
-          <t>05</t>
+          <t>04</t>
         </is>
       </c>
       <c r="C156" s="1" t="inlineStr">
@@ -5054,6 +5084,38 @@
       <c r="K156" s="1"/>
       <c r="L156" s="1"/>
     </row>
+    <row r="157">
+      <c r="A157" s="1" t="n">
+        <v>531.0</v>
+      </c>
+      <c r="B157" s="1" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
+      <c r="C157" s="1" t="inlineStr">
+        <is>
+          <t>2017</t>
+        </is>
+      </c>
+      <c r="D157" s="1"/>
+      <c r="E157" s="1"/>
+      <c r="F157" s="1"/>
+      <c r="G157" s="1" t="inlineStr">
+        <is>
+          <t>France</t>
+        </is>
+      </c>
+      <c r="H157" s="1" t="inlineStr">
+        <is>
+          <t>CORSE</t>
+        </is>
+      </c>
+      <c r="I157" s="1"/>
+      <c r="J157" s="1"/>
+      <c r="K157" s="1"/>
+      <c r="L157" s="1"/>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>